<commit_message>
Dev hwj 1111 (#334)
* 成本信息表下载完成，总经理审批、营销部审批完成

* 问题清单720、722、723、724解决

* 成本信息数据问题修改

* 仅保存功能

* 仅保存功能开发

* 报价成本信息表问题处理

* 营销部审批，成本问题处理，报价反馈增加字段

* 报价反馈相关开发

* 报价出不来的问题解决

* 文件归档报价部分完成，报价看板问题处理

* 归档完成

* 梯度走量问题解决、738改变数据结构方便前端显示，756问题解决

* 客户目标价为0引发的成本问题解决，产品名改方案，梯度走量修改

* 因为汇率为空造成的异常问题解决

* 报价流程相关处理

* 报价分析看板无法显示问题处理

* 报价分析看板处理

* 审批表问题处理

* 保存优化

* 字段控制

* 增加报价方案删除接口，总经理审批二结构修改

* 归档、样品数据问题处理

* 报价策略修改，获取数据问题处理

* 产品清单逻辑修改

* 问题处理

* 线体数量、分摊率问题解决

* 问题处理

---------

Co-authored-by: Zero656329 <hwj656329@163.com>
</commit_message>
<xml_diff>
--- a/aspnet-core/src/Finance.Web.Host/wwwroot/Excel/报价审批表模板—含样品.xlsx
+++ b/aspnet-core/src/Finance.Web.Host/wwwroot/Excel/报价审批表模板—含样品.xlsx
@@ -1425,6 +1425,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
     <xf numFmtId="176" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1469,12 +1475,6 @@
     </xf>
     <xf numFmtId="176" fontId="6" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="176" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="6">
@@ -2264,8 +2264,8 @@
   </sheetPr>
   <dimension ref="B1:V119"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
-      <selection activeCell="C24" sqref="C24:D26"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A28" zoomScale="55" zoomScaleNormal="55" workbookViewId="0">
+      <selection activeCell="E24" sqref="E24:E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.625" defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
@@ -2336,20 +2336,20 @@
       <c r="M3" s="9"/>
     </row>
     <row r="4" spans="2:19" ht="29.25" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B4" s="80" t="s">
+      <c r="B4" s="82" t="s">
         <v>107</v>
       </c>
-      <c r="C4" s="80"/>
-      <c r="D4" s="80"/>
-      <c r="E4" s="80"/>
-      <c r="F4" s="80"/>
-      <c r="G4" s="80"/>
-      <c r="H4" s="80"/>
-      <c r="I4" s="80"/>
-      <c r="J4" s="80"/>
-      <c r="K4" s="80"/>
-      <c r="L4" s="80"/>
-      <c r="M4" s="80"/>
+      <c r="C4" s="82"/>
+      <c r="D4" s="82"/>
+      <c r="E4" s="82"/>
+      <c r="F4" s="82"/>
+      <c r="G4" s="82"/>
+      <c r="H4" s="82"/>
+      <c r="I4" s="82"/>
+      <c r="J4" s="82"/>
+      <c r="K4" s="82"/>
+      <c r="L4" s="82"/>
+      <c r="M4" s="82"/>
       <c r="Q4" s="11"/>
       <c r="R4" s="11"/>
       <c r="S4" s="11"/>
@@ -2362,17 +2362,17 @@
         <v>39</v>
       </c>
       <c r="D5" s="13"/>
-      <c r="E5" s="81"/>
-      <c r="F5" s="81"/>
+      <c r="E5" s="83"/>
+      <c r="F5" s="83"/>
       <c r="G5" s="47" t="s">
         <v>1</v>
       </c>
       <c r="H5" s="48"/>
       <c r="I5" s="13"/>
-      <c r="J5" s="81"/>
-      <c r="K5" s="81"/>
-      <c r="L5" s="81"/>
-      <c r="M5" s="81"/>
+      <c r="J5" s="83"/>
+      <c r="K5" s="83"/>
+      <c r="L5" s="83"/>
+      <c r="M5" s="83"/>
     </row>
     <row r="6" spans="2:19" ht="21" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B6" s="28" t="s">
@@ -2685,19 +2685,19 @@
       <c r="M23" s="33"/>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B24" s="84" t="s">
+      <c r="B24" s="86" t="s">
         <v>13</v>
       </c>
-      <c r="C24" s="86" t="s">
+      <c r="C24" s="88" t="s">
         <v>31</v>
       </c>
-      <c r="D24" s="86" t="s">
+      <c r="D24" s="88" t="s">
         <v>32</v>
       </c>
-      <c r="E24" s="88" t="s">
+      <c r="E24" s="90" t="s">
         <v>33</v>
       </c>
-      <c r="F24" s="90" t="s">
+      <c r="F24" s="92" t="s">
         <v>34</v>
       </c>
       <c r="G24" s="14"/>
@@ -2707,11 +2707,11 @@
       <c r="K24" s="33"/>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.3">
-      <c r="B25" s="85"/>
-      <c r="C25" s="87"/>
-      <c r="D25" s="87"/>
-      <c r="E25" s="89"/>
-      <c r="F25" s="90"/>
+      <c r="B25" s="87"/>
+      <c r="C25" s="89"/>
+      <c r="D25" s="89"/>
+      <c r="E25" s="91"/>
+      <c r="F25" s="92"/>
       <c r="G25" s="14"/>
       <c r="H25" s="14"/>
       <c r="I25" s="14"/>
@@ -2860,20 +2860,20 @@
       <c r="B35" s="34" t="s">
         <v>119</v>
       </c>
-      <c r="C35" s="92" t="s">
+      <c r="C35" s="77" t="s">
         <v>115</v>
       </c>
-      <c r="D35" s="92"/>
-      <c r="E35" s="92" t="s">
+      <c r="D35" s="77"/>
+      <c r="E35" s="77" t="s">
         <v>116</v>
       </c>
-      <c r="F35" s="93" t="s">
+      <c r="F35" s="78" t="s">
         <v>117</v>
       </c>
-      <c r="G35" s="93" t="s">
+      <c r="G35" s="78" t="s">
         <v>118</v>
       </c>
-      <c r="H35" s="92"/>
+      <c r="H35" s="77"/>
       <c r="I35" s="14"/>
       <c r="J35" s="14"/>
       <c r="K35" s="14"/>
@@ -2884,23 +2884,23 @@
       <c r="B36" s="74" t="s">
         <v>74</v>
       </c>
-      <c r="C36" s="82" t="s">
+      <c r="C36" s="84" t="s">
         <v>75</v>
       </c>
-      <c r="D36" s="83"/>
+      <c r="D36" s="85"/>
       <c r="E36" s="75" t="s">
         <v>86</v>
       </c>
       <c r="F36" s="76" t="s">
         <v>76</v>
       </c>
-      <c r="G36" s="82" t="s">
+      <c r="G36" s="84" t="s">
         <v>77</v>
       </c>
-      <c r="H36" s="83"/>
-      <c r="I36" s="91"/>
-      <c r="J36" s="91"/>
-      <c r="K36" s="91"/>
+      <c r="H36" s="85"/>
+      <c r="I36" s="93"/>
+      <c r="J36" s="93"/>
+      <c r="K36" s="93"/>
       <c r="L36" s="19"/>
       <c r="M36" s="33"/>
     </row>
@@ -3067,48 +3067,48 @@
       <c r="O44" s="25"/>
     </row>
     <row r="45" spans="2:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B45" s="79" t="s">
+      <c r="B45" s="81" t="s">
         <v>48</v>
       </c>
-      <c r="C45" s="77" t="s">
+      <c r="C45" s="79" t="s">
         <v>22</v>
       </c>
-      <c r="D45" s="77" t="s">
+      <c r="D45" s="79" t="s">
         <v>17</v>
       </c>
-      <c r="E45" s="77"/>
-      <c r="F45" s="77" t="s">
+      <c r="E45" s="79"/>
+      <c r="F45" s="79" t="s">
         <v>49</v>
       </c>
-      <c r="G45" s="77"/>
-      <c r="H45" s="77" t="s">
+      <c r="G45" s="79"/>
+      <c r="H45" s="79" t="s">
         <v>50</v>
       </c>
-      <c r="I45" s="77"/>
-      <c r="J45" s="77" t="s">
+      <c r="I45" s="79"/>
+      <c r="J45" s="79" t="s">
         <v>51</v>
       </c>
-      <c r="K45" s="77"/>
-      <c r="L45" s="77" t="s">
+      <c r="K45" s="79"/>
+      <c r="L45" s="79" t="s">
         <v>18</v>
       </c>
-      <c r="M45" s="77"/>
-      <c r="N45" s="77" t="s">
+      <c r="M45" s="79"/>
+      <c r="N45" s="79" t="s">
         <v>19</v>
       </c>
-      <c r="O45" s="77"/>
-      <c r="P45" s="77" t="s">
+      <c r="O45" s="79"/>
+      <c r="P45" s="79" t="s">
         <v>52</v>
       </c>
-      <c r="Q45" s="77"/>
-      <c r="R45" s="77" t="s">
+      <c r="Q45" s="79"/>
+      <c r="R45" s="79" t="s">
         <v>20</v>
       </c>
-      <c r="S45" s="78"/>
+      <c r="S45" s="80"/>
     </row>
     <row r="46" spans="2:22" ht="19.5" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B46" s="79"/>
-      <c r="C46" s="77"/>
+      <c r="B46" s="81"/>
+      <c r="C46" s="79"/>
       <c r="D46" s="54" t="s">
         <v>53</v>
       </c>

</xml_diff>